<commit_message>
se agregan casos de prueba en codigo y documento en explorador de entidades y crea documento de informacion tecnica de red
</commit_message>
<xml_diff>
--- a/docs/test-cases/exploradorEntidades.xlsx
+++ b/docs/test-cases/exploradorEntidades.xlsx
@@ -3,6 +3,11 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dev Celsia\Automatización v2\Automatizacion\docs\test-cases\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
@@ -18,10 +23,118 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
+  <si>
+    <t>ID Caso</t>
+  </si>
+  <si>
+    <t>Nombre/ Descripcion</t>
+  </si>
+  <si>
+    <t>Tipo de prueba</t>
+  </si>
+  <si>
+    <t>Módulo</t>
+  </si>
+  <si>
+    <t>Precondiciones</t>
+  </si>
+  <si>
+    <t>Pasos a seguir</t>
+  </si>
+  <si>
+    <t>Datos de prueba</t>
+  </si>
+  <si>
+    <t>Resultado esperado</t>
+  </si>
+  <si>
+    <t>Resultado obtenido</t>
+  </si>
+  <si>
+    <t>Estado (OK/FALLA)</t>
+  </si>
+  <si>
+    <t>Automatizado</t>
+  </si>
+  <si>
+    <t>Observaciones</t>
+  </si>
+  <si>
+    <t>Positivo</t>
+  </si>
+  <si>
+    <t>El usuario debe tener permisos para acceder a la vista</t>
+  </si>
+  <si>
+    <t>OK</t>
+  </si>
+  <si>
+    <t>SI</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>CP_EXPENT_001</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ingreso a la vista Explorador de entidades</t>
+  </si>
+  <si>
+    <t>1. Clic en módulo eCenter
+2. Scroll en el contenedor de aplicaciones
+3. Clic en "Explorador de entidades"</t>
+  </si>
+  <si>
+    <t>El sistema debe redirigido correctamente la vista Explorador de entidades</t>
+  </si>
+  <si>
+    <t>La vista Explorador de entidades se cargó sin errores</t>
+  </si>
+  <si>
+    <t>CP_EXPENT_002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Selección de elemento secundario
+</t>
+  </si>
+  <si>
+    <t>CP_EXPENT_003</t>
+  </si>
+  <si>
+    <t>Crear nuevo registro
+entidad</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -37,7 +150,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -45,12 +158,104 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -69,7 +274,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -114,7 +319,7 @@
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="Yu Gothic Light"/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
         <a:font script="Hans" typeface="等线 Light"/>
         <a:font script="Hant" typeface="新細明體"/>
@@ -149,7 +354,7 @@
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="Yu Gothic"/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
         <a:font script="Hans" typeface="等线"/>
         <a:font script="Hant" typeface="新細明體"/>
@@ -331,12 +536,145 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="25" customWidth="1"/>
+    <col min="2" max="2" width="24.7109375" customWidth="1"/>
+    <col min="3" max="3" width="32.140625" customWidth="1"/>
+    <col min="4" max="5" width="28.5703125" customWidth="1"/>
+    <col min="6" max="6" width="30.7109375" customWidth="1"/>
+    <col min="7" max="7" width="30.85546875" customWidth="1"/>
+    <col min="8" max="8" width="34.42578125" customWidth="1"/>
+    <col min="9" max="9" width="38.7109375" customWidth="1"/>
+    <col min="10" max="10" width="45.28515625" customWidth="1"/>
+    <col min="11" max="11" width="69.42578125" customWidth="1"/>
+    <col min="12" max="12" width="99.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="60">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="66.75" customHeight="1">
+      <c r="A2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="K2" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="L2" s="9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="61.5" customHeight="1">
+      <c r="A3" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="10"/>
+      <c r="J3" s="10"/>
+      <c r="K3" s="10"/>
+      <c r="L3" s="10"/>
+    </row>
+    <row r="4" spans="1:12" ht="41.25" customHeight="1">
+      <c r="A4" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="11"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="10"/>
+      <c r="J4" s="10"/>
+      <c r="K4" s="10"/>
+      <c r="L4" s="10"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
se modifica documento explorador entidades
</commit_message>
<xml_diff>
--- a/docs/test-cases/exploradorEntidades.xlsx
+++ b/docs/test-cases/exploradorEntidades.xlsx
@@ -12,7 +12,7 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="ExploradorEntidades" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="31">
   <si>
     <t>ID Caso</t>
   </si>
@@ -97,22 +97,38 @@
     <t>CP_EXPENT_002</t>
   </si>
   <si>
-    <t xml:space="preserve">Selección de elemento secundario
+    <t>CP_EXPENT_003</t>
+  </si>
+  <si>
+    <t>Crear nuevo registro
+entidad(ONT)</t>
+  </si>
+  <si>
+    <t>eCenter</t>
+  </si>
+  <si>
+    <t>Debe haber accedido a la vista</t>
+  </si>
+  <si>
+    <t>1.Clic en "elemento secundario"
+2.Clic en tarjeta ONT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Selección de elemento secundario(ONT)
 </t>
   </si>
   <si>
-    <t>CP_EXPENT_003</t>
-  </si>
-  <si>
-    <t>Crear nuevo registro
-entidad</t>
+    <t>El sistema debe redirigido correctamente a los elementos secundarios (ONT)</t>
+  </si>
+  <si>
+    <t>Debe haber accedido al apartado de elemento secundario(ONT)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -132,14 +148,6 @@
       <color rgb="FF000000"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -255,7 +263,9 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -539,7 +549,7 @@
   <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -557,7 +567,7 @@
     <col min="12" max="12" width="99.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="60">
+    <row r="1" spans="1:12">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -595,7 +605,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="66.75" customHeight="1">
+    <row r="2" spans="1:12" ht="87.75" customHeight="1">
       <c r="A2" s="3" t="s">
         <v>17</v>
       </c>
@@ -606,7 +616,7 @@
         <v>12</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>13</v>
@@ -638,34 +648,48 @@
         <v>22</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
+      <c r="D3" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>29</v>
+      </c>
       <c r="I3" s="10"/>
       <c r="J3" s="10"/>
       <c r="K3" s="10"/>
       <c r="L3" s="10"/>
     </row>
-    <row r="4" spans="1:12" ht="41.25" customHeight="1">
+    <row r="4" spans="1:12" ht="66.75" customHeight="1">
       <c r="A4" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="C4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="11"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
+      <c r="E4" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F4" s="11"/>
       <c r="G4" s="10"/>
       <c r="H4" s="10"/>
       <c r="I4" s="10"/>

</xml_diff>

<commit_message>
se agregan casos de prueba en el documento explorador entidades
</commit_message>
<xml_diff>
--- a/docs/test-cases/exploradorEntidades.xlsx
+++ b/docs/test-cases/exploradorEntidades.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="44">
   <si>
     <t>ID Caso</t>
   </si>
@@ -121,7 +121,68 @@
     <t>El sistema debe redirigido correctamente a los elementos secundarios (ONT)</t>
   </si>
   <si>
-    <t>Debe haber accedido al apartado de elemento secundario(ONT)</t>
+    <t>1.Clic en la primera tarjeta
+2.Clic en botón "Nuevo registro de entidad"
+3.Diligenciar campo SERIALCELSIA con 1048XXXX
+4.Diligenciar campo FACTORYSERIAL con 485724435AXXXXXX
+5.Clic en botón Categoría
+6.Seleccionar registro ONT
+7.Clic en botón Seleccionar (confirmar categoría)
+8.Diligenciar campo IP con una dirección IPv4 aleatoria
+9.Diligenciar campo MAC con serial aleatoria
+10.Diligenciar campo Nombre con "HUAWEI_TEST"
+11.Clic en botón del campo "Modelo"
+12.digitar "EG8145V5" en la barra de búsqueda DEL MODAL
+13.Seleccionar el registro encontrado (EG8145V5)
+14.Diligenciar campo Descripción con "HUAWEI_TEST"
+15.Clic en botón del campo "Icono"
+16.Seleccionar el ícono ONT en el modal
+17.Clic en botón "Seleccionar" del modal de ícono
+18.Clic en botón del campo "Localidad"
+19.Clic en botón "Seleccionar" del modal de Localidad.
+20.Clic en la flecha "Siguiente" en el formulario de creación de entidad.
+21.Clic en botón "Crear" y esperar finalización del progreso</t>
+  </si>
+  <si>
+    <t>La vista de los elementos secundarios(ONT) se cargó sin errores</t>
+  </si>
+  <si>
+    <t>El sistema debe crear un registro de entidad (ONT)</t>
+  </si>
+  <si>
+    <t>CP_EXPENT_004</t>
+  </si>
+  <si>
+    <t>Eliminar registro
+entidad(ONT)</t>
+  </si>
+  <si>
+    <t>Debe haber accedido al apartado de elemento secundario(ONT) y seleccionado una ont</t>
+  </si>
+  <si>
+    <t>Debe haber seleccionado un elemento secundario(ONT)</t>
+  </si>
+  <si>
+    <t>El sistema debe eliminar el registro seleccionado de entidad (ONT)</t>
+  </si>
+  <si>
+    <t>El  registro de entidad (ONT) se creo exitosamente</t>
+  </si>
+  <si>
+    <t>CP_EXPENT_005</t>
+  </si>
+  <si>
+    <t>Editar registro
+entidad(ONT)</t>
+  </si>
+  <si>
+    <t>El sistema debe editar el registro de entidad (ONT) seleccionado</t>
+  </si>
+  <si>
+    <t>El  registro de entidad (ONT) se editó exitosamente</t>
+  </si>
+  <si>
+    <t>El  registro de entidad (ONT) se eliminó exitosamente</t>
   </si>
 </sst>
 </file>
@@ -233,7 +294,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -262,7 +323,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -546,10 +606,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -558,7 +618,7 @@
     <col min="2" max="2" width="24.7109375" customWidth="1"/>
     <col min="3" max="3" width="32.140625" customWidth="1"/>
     <col min="4" max="5" width="28.5703125" customWidth="1"/>
-    <col min="6" max="6" width="30.7109375" customWidth="1"/>
+    <col min="6" max="6" width="46.7109375" customWidth="1"/>
     <col min="7" max="7" width="30.85546875" customWidth="1"/>
     <col min="8" max="8" width="34.42578125" customWidth="1"/>
     <col min="9" max="9" width="38.7109375" customWidth="1"/>
@@ -656,7 +716,7 @@
       <c r="D3" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="E3" s="10" t="s">
         <v>26</v>
       </c>
       <c r="F3" s="4" t="s">
@@ -668,12 +728,20 @@
       <c r="H3" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="I3" s="10"/>
-      <c r="J3" s="10"/>
-      <c r="K3" s="10"/>
-      <c r="L3" s="10"/>
+      <c r="I3" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="K3" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="L3" s="9" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="4" spans="1:12" ht="66.75" customHeight="1">
+    <row r="4" spans="1:12" ht="104.25" customHeight="1">
       <c r="A4" s="3" t="s">
         <v>23</v>
       </c>
@@ -687,15 +755,101 @@
         <v>25</v>
       </c>
       <c r="E4" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="F4" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="F4" s="11"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="10"/>
-      <c r="I4" s="10"/>
-      <c r="J4" s="10"/>
-      <c r="K4" s="10"/>
-      <c r="L4" s="10"/>
+      <c r="G4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="K4" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="L4" s="9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="104.25" customHeight="1">
+      <c r="A5" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F5" s="4"/>
+      <c r="G5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="K5" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="L5" s="9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="104.25" customHeight="1">
+      <c r="A6" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F6" s="4"/>
+      <c r="G6" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="J6" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="K6" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="L6" s="9" t="s">
+        <v>16</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
se agrega el caso de prueba CP_EXPENT_004 en explorador de entidades
</commit_message>
<xml_diff>
--- a/docs/test-cases/exploradorEntidades.xlsx
+++ b/docs/test-cases/exploradorEntidades.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29231"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dev Celsia\Automatizacion\docs\test-cases\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dev Celsia\Automatización v2\Automatizacion\docs\test-cases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E937F6A9-6DAF-413B-B4B3-DD97EE61DC5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720"/>
   </bookViews>
   <sheets>
     <sheet name="ExploradorEntidades" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="45">
   <si>
     <t>ID Caso</t>
   </si>
@@ -122,10 +121,51 @@
     <t>El sistema debe redirigido correctamente a los elementos secundarios (ONT)</t>
   </si>
   <si>
+    <t>La vista de los elementos secundarios(ONT) se cargó sin errores</t>
+  </si>
+  <si>
+    <t>El sistema debe crear un registro de entidad (ONT)</t>
+  </si>
+  <si>
+    <t>CP_EXPENT_004</t>
+  </si>
+  <si>
+    <t>Eliminar registro
+entidad(ONT)</t>
+  </si>
+  <si>
+    <t>Debe haber accedido al apartado de elemento secundario(ONT) y seleccionado una ont</t>
+  </si>
+  <si>
+    <t>Debe haber seleccionado un elemento secundario(ONT)</t>
+  </si>
+  <si>
+    <t>El sistema debe eliminar el registro seleccionado de entidad (ONT)</t>
+  </si>
+  <si>
+    <t>El  registro de entidad (ONT) se creo exitosamente</t>
+  </si>
+  <si>
+    <t>CP_EXPENT_005</t>
+  </si>
+  <si>
+    <t>Editar registro
+entidad(ONT)</t>
+  </si>
+  <si>
+    <t>El sistema debe editar el registro de entidad (ONT) seleccionado</t>
+  </si>
+  <si>
+    <t>El  registro de entidad (ONT) se editó exitosamente</t>
+  </si>
+  <si>
+    <t>El  registro de entidad (ONT) se eliminó exitosamente</t>
+  </si>
+  <si>
     <t>1.Clic en la primera tarjeta
 2.Clic en botón "Nuevo registro de entidad"
 3.Diligenciar campo SERIALCELSIA con 1048XXXX
-4.Diligenciar campo FACTORYSERIAL con 485724435AXXXXXX
+4.Diligenciar campo FACTORYSERIAL con 4.5724435AXXXXXX
 5.Clic en botón Categoría
 6.Seleccionar registro ONT
 7.Clic en botón Seleccionar (confirmar categoría)
@@ -145,52 +185,15 @@
 21.Clic en botón "Crear" y esperar finalización del progreso</t>
   </si>
   <si>
-    <t>La vista de los elementos secundarios(ONT) se cargó sin errores</t>
-  </si>
-  <si>
-    <t>El sistema debe crear un registro de entidad (ONT)</t>
-  </si>
-  <si>
-    <t>CP_EXPENT_004</t>
-  </si>
-  <si>
-    <t>Eliminar registro
-entidad(ONT)</t>
-  </si>
-  <si>
-    <t>Debe haber accedido al apartado de elemento secundario(ONT) y seleccionado una ont</t>
-  </si>
-  <si>
-    <t>Debe haber seleccionado un elemento secundario(ONT)</t>
-  </si>
-  <si>
-    <t>El sistema debe eliminar el registro seleccionado de entidad (ONT)</t>
-  </si>
-  <si>
-    <t>El  registro de entidad (ONT) se creo exitosamente</t>
-  </si>
-  <si>
-    <t>CP_EXPENT_005</t>
-  </si>
-  <si>
-    <t>Editar registro
-entidad(ONT)</t>
-  </si>
-  <si>
-    <t>El sistema debe editar el registro de entidad (ONT) seleccionado</t>
-  </si>
-  <si>
-    <t>El  registro de entidad (ONT) se editó exitosamente</t>
-  </si>
-  <si>
-    <t>El  registro de entidad (ONT) se eliminó exitosamente</t>
+    <t>1.Seleccionar la barra de búsqueda y digitar "HUAWEI TEST"
+2.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -606,14 +609,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="25" customWidth="1"/>
     <col min="2" max="2" width="24.7109375" customWidth="1"/>
@@ -628,7 +631,7 @@
     <col min="12" max="12" width="23.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -666,7 +669,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="87.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="87.75" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>17</v>
       </c>
@@ -704,7 +707,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="61.5" customHeight="1">
       <c r="A3" s="1" t="s">
         <v>22</v>
       </c>
@@ -730,7 +733,7 @@
         <v>29</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J3" s="3" t="s">
         <v>14</v>
@@ -742,7 +745,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="104.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" ht="104.25" customHeight="1">
       <c r="A4" s="1" t="s">
         <v>23</v>
       </c>
@@ -756,19 +759,19 @@
         <v>25</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>16</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J4" s="3" t="s">
         <v>14</v>
@@ -780,12 +783,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="104.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" ht="104.25" customHeight="1">
       <c r="A5" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>12</v>
@@ -794,17 +797,19 @@
         <v>25</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="F5" s="2"/>
+        <v>35</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>44</v>
+      </c>
       <c r="G5" s="1" t="s">
         <v>16</v>
       </c>
       <c r="H5" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I5" s="1" t="s">
         <v>41</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>42</v>
       </c>
       <c r="J5" s="3" t="s">
         <v>14</v>
@@ -816,12 +821,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="104.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" ht="104.25" customHeight="1">
       <c r="A6" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>12</v>
@@ -830,17 +835,17 @@
         <v>25</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="1" t="s">
         <v>16</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J6" s="3" t="s">
         <v>14</v>

</xml_diff>